<commit_message>
Lab & workshops + setup
</commit_message>
<xml_diff>
--- a/references/Ideas.xlsx
+++ b/references/Ideas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Personal)\Solliance\microsoft-data-engineering-ilt\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7706814-EE40-4B97-8F37-EA42245D21BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84807364-2429-497A-A23B-84550AD5666E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35290" yWindow="5150" windowWidth="12190" windowHeight="8380" firstSheet="1" activeTab="9" xr2:uid="{6BB2C407-E14E-44AD-ADA1-2327FC5C0B1E}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" firstSheet="1" activeTab="9" xr2:uid="{6BB2C407-E14E-44AD-ADA1-2327FC5C0B1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Exam OD list" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Labs to modules mapping" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="441">
   <si>
     <t>Design and Implement Data Storage  41%</t>
   </si>
@@ -4433,21 +4434,9 @@
     <t>Lab(s)</t>
   </si>
   <si>
-    <t>Lab 1: Perform Data Engineering and exploration (github.com)</t>
-  </si>
-  <si>
     <t>Databricks-demo workspace: MS_Learn_Final/11-Delta-Lake-Architecture/1-Delta-Architecture (https://github.com/solliancenet/microsoft-learning-paths-databricks-notebooks/blob/master/data-engineering/DBC/11-Delta-Lake-Architecture.dbc)</t>
   </si>
   <si>
-    <t>azure-synapse-analytics-ga-content-packs/README.md at main · solliancenet/azure-synapse-analytics-ga-content-packs (github.com)</t>
-  </si>
-  <si>
-    <t>synapse-training/README.md at main · solliancenet/synapse-training (github.com)</t>
-  </si>
-  <si>
-    <t>tech-immersion-data-ai/README.md at master · solliancenet/tech-immersion-data-ai (github.com)</t>
-  </si>
-  <si>
     <t>(Use the vehicle telemetry generator executable from experience 6 instead of requiring Visual Studio: https://github.com/solliancenet/tech-immersion-data-ai/blob/master/data-exp6/README.md)</t>
   </si>
   <si>
@@ -4470,6 +4459,54 @@
   </si>
   <si>
     <t>microsoft-learning-paths-databricks-update/data-engineering-with-azure-databricks/04-work-with-dataframes-in-azure-databricks at master · solliancenet/microsoft-learning-paths-databricks-update (github.com)</t>
+  </si>
+  <si>
+    <t>Sanjay whiteboard and/or L400 whiteboards</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/synapse-training/blob/main/labs/day1/lab3/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/synapse-training/blob/main/labs/day1/lab1/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/synapse-training/blob/main/labs/day1/lab2/README.md</t>
+  </si>
+  <si>
+    <t>(bottom part of lab)</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/synapse-training/blob/main/labs/day1/lab4/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/synapse-training/tree/main/labs/day2/lab1</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/synapse-training/blob/main/labs/day2/lab2/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/tech-immersion-data-ai/blob/master/data-exp4/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/tech-immersion-data-ai/blob/master/data-exp6/README.md</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/azure-synapse-analytics-ga-content-packs/blob/main/hands-on-labs/lab-02/README.md#task-2---index-the-data-lake-storage-with-hyperspace</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/azure-synapse-analytics-ga-content-packs/tree/main/hands-on-labs/lab-01</t>
+  </si>
+  <si>
+    <t>Azure ML integrated with Synapse (the recommended way)</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/synapse-training/tree/main/labs/day2/lab5</t>
+  </si>
+  <si>
+    <t>(replace with HTAP)</t>
+  </si>
+  <si>
+    <t>https://github.com/solliancenet/microsoft-learning-paths-databricks-update/tree/master/data-engineering-with-azure-databricks/10-process-streaming-data-with-azure-databricks-structured-streaming</t>
   </si>
 </sst>
 </file>
@@ -5586,10 +5623,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8057CCF5-3012-4834-B02F-49AFE5E6BA65}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -5608,141 +5645,187 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B3" s="18" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A5" s="12"/>
+      <c r="B5" s="18" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B4" s="18" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="12">
-        <v>2</v>
-      </c>
-      <c r="B5" s="18" t="s">
+      <c r="B6" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="18" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>438</v>
+      </c>
+      <c r="G7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>426</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="12">
-        <v>4</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="18" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>419</v>
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A11">
-        <v>5</v>
-      </c>
       <c r="B11" s="18" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B12" s="18" t="s">
-        <v>419</v>
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>419</v>
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>428</v>
+      </c>
+      <c r="G14" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>433</v>
+      </c>
+      <c r="G18" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="G19" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="G20" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>440</v>
+      </c>
+      <c r="G21" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
         <v>420</v>
       </c>
-      <c r="G14" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="G15" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="G16" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A18">
-        <v>9</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>424</v>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>436</v>
+      </c>
+      <c r="G23" t="s">
+        <v>437</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/solliancenet/synapse-training/blob/main/labs/day1/lab1/README.md" xr:uid="{C30EC9B7-8E02-4014-AB17-360DA5CAA1BC}"/>
-    <hyperlink ref="B4" r:id="rId2" location="task-2---index-the-data-lake-storage-with-hyperspace" display="task-2---index-the-data-lake-storage-with-hyperspace" xr:uid="{D6367AB5-9F41-4534-AA56-3982BDAC046A}"/>
-    <hyperlink ref="B9" r:id="rId3" display="https://github.com/solliancenet/synapse-training/blob/main/labs/day1/lab2/README.md" xr:uid="{578276E1-95B6-434D-8F95-7D32876D0AC1}"/>
-    <hyperlink ref="B10" r:id="rId4" display="https://github.com/solliancenet/synapse-training/blob/main/labs/day1/lab3/README.md" xr:uid="{8502C612-C7C2-49BB-9327-C7F129C93810}"/>
-    <hyperlink ref="B11" r:id="rId5" display="https://github.com/solliancenet/synapse-training/blob/main/labs/day1/lab4/README.md" xr:uid="{31023CC9-6B23-4B4E-9713-80108D5209E9}"/>
-    <hyperlink ref="B12" r:id="rId6" display="https://github.com/solliancenet/synapse-training/blob/main/labs/day2/lab1/README.md" xr:uid="{36DCA99F-9224-475B-B317-74F3D587AF66}"/>
-    <hyperlink ref="B13" r:id="rId7" display="https://github.com/solliancenet/synapse-training/blob/main/labs/day2/lab2/README.md" xr:uid="{84762563-01C9-425C-BCD0-E2E12F613EEA}"/>
-    <hyperlink ref="B14" r:id="rId8" display="https://github.com/solliancenet/tech-immersion-data-ai/blob/master/data-exp4/README.md" xr:uid="{C0DD8BBC-2860-4CCF-9144-79A412CD7B87}"/>
-    <hyperlink ref="B17" r:id="rId9" display="https://github.com/solliancenet/tech-immersion-data-ai/blob/master/data-exp6/README.md" xr:uid="{E4909B8B-2EC4-4783-ACC9-046E10D33994}"/>
-    <hyperlink ref="B18" r:id="rId10" xr:uid="{B7CA8A4B-6007-4876-82D2-08489811BFE8}"/>
-    <hyperlink ref="B5" r:id="rId11" xr:uid="{D9786BA1-63F0-4D5C-BD60-0A846108D21E}"/>
-    <hyperlink ref="B6" r:id="rId12" display="https://www.dropbox.com/s/jlgg4wp9o5x92j0/Mod 11 - SSAS -Beginning MultiDimensional.zip?dl=0" xr:uid="{20310025-76DA-4C68-AEB0-128505E4E915}"/>
-    <hyperlink ref="B7" r:id="rId13" display="https://github.com/solliancenet/microsoft-learning-paths-databricks-update/tree/master/data-engineering-with-azure-databricks/07-work-with-dataframe-advanced-methods-in-azure-databricks" xr:uid="{7D051C15-1DD2-4716-8524-7BAE82CA79CE}"/>
-    <hyperlink ref="B8" r:id="rId14" display="https://github.com/solliancenet/microsoft-learning-paths-databricks-update/tree/master/data-engineering-with-azure-databricks/04-work-with-dataframes-in-azure-databricks" xr:uid="{A07476AA-6447-48FC-BC45-42F504102B1F}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{D9786BA1-63F0-4D5C-BD60-0A846108D21E}"/>
+    <hyperlink ref="B5" r:id="rId2" display="https://www.dropbox.com/s/jlgg4wp9o5x92j0/Mod 11 - SSAS -Beginning MultiDimensional.zip?dl=0" xr:uid="{20310025-76DA-4C68-AEB0-128505E4E915}"/>
+    <hyperlink ref="B10" r:id="rId3" display="https://github.com/solliancenet/microsoft-learning-paths-databricks-update/tree/master/data-engineering-with-azure-databricks/07-work-with-dataframe-advanced-methods-in-azure-databricks" xr:uid="{7D051C15-1DD2-4716-8524-7BAE82CA79CE}"/>
+    <hyperlink ref="B11" r:id="rId4" display="https://github.com/solliancenet/microsoft-learning-paths-databricks-update/tree/master/data-engineering-with-azure-databricks/04-work-with-dataframes-in-azure-databricks" xr:uid="{A07476AA-6447-48FC-BC45-42F504102B1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
UI updates and clarification of some steps
</commit_message>
<xml_diff>
--- a/references/Ideas.xlsx
+++ b/references/Ideas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Personal)\Solliance\microsoft-data-engineering-ilt\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22B4488-CD90-44AE-967D-A346840CD998}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FA542D-7542-4D8B-BAF1-1B2584217E51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" firstSheet="1" activeTab="9" xr2:uid="{6BB2C407-E14E-44AD-ADA1-2327FC5C0B1E}"/>
   </bookViews>
@@ -5625,7 +5625,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -5772,7 +5772,7 @@
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="18" t="s">
         <v>433</v>
       </c>
       <c r="G18" t="s">
@@ -5825,6 +5825,7 @@
     <hyperlink ref="B5" r:id="rId2" display="https://www.dropbox.com/s/jlgg4wp9o5x92j0/Mod 11 - SSAS -Beginning MultiDimensional.zip?dl=0" xr:uid="{20310025-76DA-4C68-AEB0-128505E4E915}"/>
     <hyperlink ref="B9" r:id="rId3" display="https://github.com/solliancenet/microsoft-learning-paths-databricks-update/tree/master/data-engineering-with-azure-databricks/07-work-with-dataframe-advanced-methods-in-azure-databricks" xr:uid="{7D051C15-1DD2-4716-8524-7BAE82CA79CE}"/>
     <hyperlink ref="B10" r:id="rId4" display="https://github.com/solliancenet/microsoft-learning-paths-databricks-update/tree/master/data-engineering-with-azure-databricks/04-work-with-dataframes-in-azure-databricks" xr:uid="{A07476AA-6447-48FC-BC45-42F504102B1F}"/>
+    <hyperlink ref="B18" r:id="rId5" xr:uid="{FA7B2EF0-1944-4B71-A1CF-E9555C905F25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>